<commit_message>
feat: added snapping charts
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,44 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grego\Documents\upwork\014_dashboard\var_dashboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A1D9C7-A3B9-4CEB-B62F-669FCA9776BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>some text</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>var_structured_position_top10</t>
+  </si>
+  <si>
+    <t>fund_exp_pct_dashboard</t>
+  </si>
+  <si>
+    <t>sector_exposure_df</t>
+  </si>
+  <si>
+    <t>var_structured_position_bottom10</t>
+  </si>
+  <si>
+    <t>fund_exp_usd_dashboard</t>
+  </si>
+  <si>
+    <t>something_else</t>
+  </si>
+  <si>
+    <t>another thing</t>
+  </si>
+  <si>
+    <t>another thing to the left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,27 +87,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F7" totalsRowShown="0">
-  <autoFilter ref="B3:F7"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -133,7 +139,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -167,6 +173,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -201,9 +208,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -376,42 +384,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
-      <c r="B1" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>